<commit_message>
Update that allows cobb-douglas in CES class
</commit_message>
<xml_diff>
--- a/InputDisplacingAbatement/Make_data/FinalGoods.xlsx
+++ b/InputDisplacingAbatement/Make_data/FinalGoods.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mu" sheetId="1" r:id="rId1"/>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with a simulation in example1
</commit_message>
<xml_diff>
--- a/InputDisplacingAbatement/Make_data/FinalGoods.xlsx
+++ b/InputDisplacingAbatement/Make_data/FinalGoods.xlsx
@@ -514,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>